<commit_message>
Reg fetch, inst decode, and r-type states and updating alu control and ALUOp signal
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1375B5F-CBA1-45BB-977E-0010A182F1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05D2395-0473-4452-A2E1-55EF16C4C84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,22 @@
 - Only need Quartus to get RAM IP file as far as I can tell. And for full synthesis
 Bugs
 - N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- Made a couple of comments (night of 8/14/25)                                                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- ALUOp: Changed ALUOp to be the same as IR31to26 aka the OP Code (updated top_level, Datapath, Controller, and alu_control entities)
+- CONTROLLER: Added and defined REG_FETCH, INST_DECODE, and R_TYPE states         
+- ALU CONTROL: Added case for ADD 4 to PC, R-type inst, and ADDU inst                                                                                                                                                                                                                                </t>
+  </si>
+  <si>
+    <t>Notes
+- Don't think I need to use any kind of states in ALU Control
+Bugs
+- Haven't tested any of this yet but it compiles</t>
   </si>
 </sst>
 </file>
@@ -422,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,10 +496,10 @@
     </row>
     <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>45876</v>
+        <v>45884</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
@@ -492,24 +508,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>45877</v>
+        <v>45885</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>45878</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -521,9 +535,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>45879</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
@@ -535,9 +547,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>45880</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -545,6 +555,28 @@
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added testbenches for alu_control and Controller and tested them
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05D2395-0473-4452-A2E1-55EF16C4C84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2014BBD2-1C83-4F1A-A1F5-798E651E81FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Change Log" sheetId="1" r:id="rId1"/>
+    <sheet name="VHDL Entities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -104,16 +105,111 @@
   <si>
     <t>Notes
 - Don't think I need to use any kind of states in ALU Control
+- NEXT STEP: Make controller/alu_control testbench
 Bugs
 - Haven't tested any of this yet but it compiles</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Tested with Testbench</t>
+  </si>
+  <si>
+    <t>alu</t>
+  </si>
+  <si>
+    <t>alu_control</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Datapath</t>
+  </si>
+  <si>
+    <t>enable_logic</t>
+  </si>
+  <si>
+    <t>Memory_top_level</t>
+  </si>
+  <si>
+    <t>mux2to1</t>
+  </si>
+  <si>
+    <t>mux4to1</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>registerfile</t>
+  </si>
+  <si>
+    <t>sign_extend</t>
+  </si>
+  <si>
+    <t>top_level</t>
+  </si>
+  <si>
+    <t>Testbenches</t>
+  </si>
+  <si>
+    <t>tb_sign_extend</t>
+  </si>
+  <si>
+    <t>tb_Memory_top_level</t>
+  </si>
+  <si>
+    <t>tb_top_level</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>tb_alu</t>
+  </si>
+  <si>
+    <t>tb_alu_control</t>
+  </si>
+  <si>
+    <t>tb_Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- Added testbenches tb_alu_control and tb_Controller for the alu_control and Controller, respectively. Tested out using these testbenches                                                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Decided on using the .mif file for integration testing and unit testbenches for unit testing
+- NEXT STEPS: Continue w/ simple R-types in alu_control. Skip to an I-type like addi so can load regfile with stuff. Test: Integration testing with .mif &amp; unit testing with unit testbenches
+Bugs
+- </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,6 +253,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,16 +621,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+    <row r="6" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>45886</v>
+      </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -583,4 +684,178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B7F85F-579F-433C-BABB-104A458DD3F3}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added AND, OR, XOR, and shift ops to alu_control and alu
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2014BBD2-1C83-4F1A-A1F5-798E651E81FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5CBAD6-5459-4D50-883C-0B324511ED53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,17 @@
     <t xml:space="preserve">Notes
 - Decided on using the .mif file for integration testing and unit testbenches for unit testing
 - NEXT STEPS: Continue w/ simple R-types in alu_control. Skip to an I-type like addi so can load regfile with stuff. Test: Integration testing with .mif &amp; unit testing with unit testbenches
+Bugs
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: alu_control.vhd, alu.vhd
+- ADDED: AND, OR, XOR, Shift right and left logical, and shift right arithmetic                                                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Haven't tested what you added to alu_control or alu yet, but it all compiles so far
 Bugs
 - </t>
   </si>
@@ -539,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,15 +647,17 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3">
+        <v>45886</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added slt and sltu to alu_control and alu
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5CBAD6-5459-4D50-883C-0B324511ED53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DAC8F4-9464-4F35-AE2B-52A3025E42D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -203,6 +203,20 @@
   <si>
     <t xml:space="preserve">Notes
 - Haven't tested what you added to alu_control or alu yet, but it all compiles so far
+Bugs
+- </t>
+  </si>
+  <si>
+    <t>Night of 8/20/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: alu_control.vhd, alu.vhd
+- ADDED: Set on less than signed and unsigned                                                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Compiles
 Bugs
 - </t>
   </si>
@@ -550,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,15 +675,17 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Verified encodings in MyMIF.mif and added comments to it
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC65651-6160-4BC2-9564-D22A322C592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A99DDD-E454-4554-87D7-0E00B6BB272B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -246,6 +246,17 @@
     <t xml:space="preserve">Changes
 - MODIFIED: MyMIF.mif, top_level.vhd, GitHub repo
 - ADDED: Comments, Issues (to GitHub repo)                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Likely could've had ChatGPT do this as you did have it get the instruction encodings in the 1st place. But it failed when you attempted to ask it to verify them, so I verified them myself.
+Bugs
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif
+- ADDED: Verified encodings and added verification comments                                                                                                                                                                                                                                     </t>
   </si>
 </sst>
 </file>
@@ -591,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,16 +768,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>45941</v>
+      </c>
       <c r="B12" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tested (simulated) all instructions in MyMIF.mif and added comments to reflect that
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A99DDD-E454-4554-87D7-0E00B6BB272B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24100E40-FBC9-49D6-950F-3452F8BA0D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -257,6 +257,11 @@
     <t xml:space="preserve">Changes
 - MODIFIED: MyMIF.mif
 - ADDED: Verified encodings and added verification comments                                                                                                                                                                                                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif
+- COMPLETED: Testing (simulation) for all instructions currently in the file. Added comments about said testing.                                                                                                                                                                                                                                       </t>
   </si>
 </sst>
 </file>
@@ -602,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,9 +788,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3">
+        <v>45942</v>
+      </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Implemented the rest of the I-type instructions. Tested up to XORI w/ MyMIF.mif. Have not tested SLTI or SLTIU yet
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24100E40-FBC9-49D6-950F-3452F8BA0D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FE2EE9-7775-4CC2-808B-3255C32C5E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1476" windowWidth="21312" windowHeight="11652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change Log" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -262,6 +262,33 @@
     <t xml:space="preserve">Changes
 - MODIFIED: MyMIF.mif
 - COMPLETED: Testing (simulation) for all instructions currently in the file. Added comments about said testing.                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- ANDI, ORI, XORI simulated/tested. I'm thinking you could try to finish most if not all of the rest of the I-type instructions before simulating/testing them
+Bugs
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: Controller.vhd, alu_control.vhd, MyMIF.mif
+- ADDED: Instructions ANDI, ORI, and XORI to all said files                                                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: Controller.vhd, alu_control.vhd
+- STARTED: Started adding STLI stuff but had to stop mid-way through so it was incomplete and may be wrong lol                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: Controller.vhd, alu_control.vhd
+- ADDED: Finished STLI and added STLIU to said files                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Have not tested STLI or STLIU yet. Also haven't watched video part on them yet. Pretty sure you stopped at about the 10 min mark of video 19 last time
+Bugs
+- </t>
   </si>
 </sst>
 </file>
@@ -607,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,22 +828,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>45946</v>
+      </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3">
+        <v>45950</v>
+      </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>3</v>
@@ -825,16 +856,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>45954</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implemented LW & SW. Added instructions to MyMIF.mif to test LW & SW. Haven't actually tested LW or SW yet
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FE2EE9-7775-4CC2-808B-3255C32C5E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B0BCF5-FC72-4CE7-97D8-41E120B0DB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1476" windowWidth="21312" windowHeight="11652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change Log" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -287,6 +287,17 @@
   <si>
     <t xml:space="preserve">Notes
 - Have not tested STLI or STLIU yet. Also haven't watched video part on them yet. Pretty sure you stopped at about the 10 min mark of video 19 last time
+Bugs
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif, Controller.vhd, alu_control.vhd
+- ADDED: Instructions to test SLTI, SLTIU, LW, and SW in MyMIF.mif. Implemented LW &amp; SW in Controller.vhd/alu_control.vhd                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Tested SLTI/SLTIU and they work. Haven't tested LW/SW yet but have the instructions ready to test in MyMIF.mif. May also need to look at the thing that tells you how to use the memory viewer thing in ModelSim. Stopped at around 36:30 in video 19 as well. He had finished LW/SW and was about to go into jump/branch instructions.
 Bugs
 - </t>
   </si>
@@ -635,7 +646,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,16 +881,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>45954</v>
+      </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tested LW & SW. Changed addressing so Program Counter is incremented by 1 instead of 4 each time. Makes adressing with LW & SW more intuitive in my opinion
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B0BCF5-FC72-4CE7-97D8-41E120B0DB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A680ED66-1026-425B-BE0F-838B3F40648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,17 @@
 - Tested SLTI/SLTIU and they work. Haven't tested LW/SW yet but have the instructions ready to test in MyMIF.mif. May also need to look at the thing that tells you how to use the memory viewer thing in ModelSim. Stopped at around 36:30 in video 19 as well. He had finished LW/SW and was about to go into jump/branch instructions.
 Bugs
 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif, Memory_top_level.vhd, Datapath.vhd
+- COMPLETED: Tested LW &amp; SW. Changed the RAM port mapping in Memory_top_level from 9 downto 2 to 7 downto 0. Changed the ALU input B MUX hard coded input value from 0x4 to 0x1                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t>Notes
+- Made changes to old files that you hadn't touched in a while. Everything still seems to work as expected so far.
+Bugs
+- I thought there was a bug with the addressing, but I just didn't realize that you needed to shift the address to the left by 2. So, I made it more intuitive in my opinion where you don't have to do that, and that is described in the Changes cell to the left.</t>
   </si>
 </sst>
 </file>
@@ -645,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,16 +906,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
+    <row r="18" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>45955</v>
+      </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implemented & tested Jump and Jump Register instructions. Modified datapath as a result of using your different addressing method
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A680ED66-1026-425B-BE0F-838B3F40648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CECCE2-76F2-437E-8432-6FE1F0E6B7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -311,6 +311,17 @@
 - Made changes to old files that you hadn't touched in a while. Everything still seems to work as expected so far.
 Bugs
 - I thought there was a bug with the addressing, but I just didn't realize that you needed to shift the address to the left by 2. So, I made it more intuitive in my opinion where you don't have to do that, and that is described in the Changes cell to the left.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif, Datapath.vhd, alu.vhd, alu_control.vhd, Controller.vhd
+- COMPLETED: Tested J &amp; JR instructions. Changed datapath for J instruction because of your different addressing method. Added stuff for J &amp; JR to alu.vhd, alu_control.vhd, and Controller.vhd                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- In vid, he said MIPS is byte-addressible so might have to do the 9 downto 2 thing for that which wouldn't be a problem. But I'm just not gonna do it that way lol. So far it seems like your way of doing the addressing is working.
+Bugs
+- </t>
   </si>
 </sst>
 </file>
@@ -654,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,16 +931,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>45956</v>
+      </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -941,6 +954,90 @@
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented & tested JAL. Added a comment to registerfile.vhd
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CECCE2-76F2-437E-8432-6FE1F0E6B7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C6F091-D291-495A-9B9B-BEFD71F04940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -322,6 +322,11 @@
 - In vid, he said MIPS is byte-addressible so might have to do the 9 downto 2 thing for that which wouldn't be a problem. But I'm just not gonna do it that way lol. So far it seems like your way of doing the addressing is working.
 Bugs
 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif, alu.vhd, alu_control.vhd, Controller.vhd, registerfile.vhd
+- COMPLETED: Implemented &amp; tested JAL instruction. Added a comment to registerfile.vhd                                                                                                                                                                                                                                       </t>
   </si>
 </sst>
 </file>
@@ -668,7 +673,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,9 +951,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
+      <c r="A20" s="3">
+        <v>45956</v>
+      </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Implemented all of the branch instructions. Only tested BEQ so far. I'm really close to actually being done, and I am practically done so...YAYYYYY!!!
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C6F091-D291-495A-9B9B-BEFD71F04940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8528213E-40D9-447C-BBA1-800B625858B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="VHDL Entities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -327,6 +328,24 @@
     <t xml:space="preserve">Changes
 - MODIFIED: MyMIF.mif, alu.vhd, alu_control.vhd, Controller.vhd, registerfile.vhd
 - COMPLETED: Implemented &amp; tested JAL instruction. Added a comment to registerfile.vhd                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- Stopped at about min 27 of vid 20. My implementation uses an extra cycle than needed, which I found out from the video pretty much
+Bugs
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif, alu.vhd, alu_control.vhd, Controller.vhd         
+- COMPLETED: Implemented all the branch instructions (BEQ, BNE, BLEZ, BGEZ, BLTZ, BGTZ). Only tested BEQ in the .mif file so far                                                                                                                                                                                                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- I have only tested BEQ so far, but all of the branch instructions are very similar so I expect the rest of them to work as well. After the initial instruction decode state in the controller, I was able to implement with only 1 other branch state after initially making different states for each instruction
+- I mean tbh the only thing that's really left is to test the rest of the branch instructions, which I highly expect to work. So really I'm pretty much done lol. YAYYYYY!!!
+Bugs
+- </t>
   </si>
 </sst>
 </file>
@@ -673,7 +692,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,7 +969,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45956</v>
       </c>
@@ -961,19 +980,21 @@
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>45958</v>
+      </c>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Finished! YAYYYYY!!! I finished testing the branch instructions in MyMIF.mif. I also used the provided files to test as well but I did have to change them a little bit because of how I do addressing slightly different
</commit_message>
<xml_diff>
--- a/Change_Log.xlsx
+++ b/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahw\Docs_notSaved\EEL4712C\MIPS\Weeks_All\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8528213E-40D9-447C-BBA1-800B625858B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1489ED-BD22-4B05-9734-7F88407F7262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="VHDL Entities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -344,6 +343,18 @@
     <t xml:space="preserve">Notes
 - I have only tested BEQ so far, but all of the branch instructions are very similar so I expect the rest of them to work as well. After the initial instruction decode state in the controller, I was able to implement with only 1 other branch state after initially making different states for each instruction
 - I mean tbh the only thing that's really left is to test the rest of the branch instructions, which I highly expect to work. So really I'm pretty much done lol. YAYYYYY!!!
+Bugs
+- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes
+- MODIFIED: MyMIF.mif, Deliverable4.mif, TestCase7.mif
+- COMPLETED: Finished testing all of the branch instructions using MyMIF.mif. Then tested with Deliverable4.mif and TestCase7.mif. Changed some things in those .mif files because of my design change to addressing. So everything works but some of the instructions work differently because of how I use addresses, but I could definitely change that so it works as intended. And the things with inport and outport don't work because it isn't running on an actual board                                                                                                                                                                                                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes
+- I did further change TestCase7.mif so it fits with my addressing so that it works as expected. The only part that doesn't work now is writing/reading to and from the outport/inport(s), but that was to be expected, as I wasn't planning on implementing that
+- I guess I'm done now lol. YAYYYYY!!!
 Bugs
 - </t>
   </si>
@@ -691,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -997,16 +1008,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
+    <row r="22" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>45958</v>
+      </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">

</xml_diff>